<commit_message>
add test case 장바구니
</commit_message>
<xml_diff>
--- a/api-test-pipeline-web 테스트케이스.xlsx
+++ b/api-test-pipeline-web 테스트케이스.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace2020\2021-web\api-test-pipeline-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFFA53A-E1D0-4EEE-9244-57CF440A7D5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6A48A-4CD8-4326-87C1-355CFC2D4ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821AE999-F993-420C-A6D8-1131BD503D21}"/>
+    <workbookView xWindow="34860" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{821AE999-F993-420C-A6D8-1131BD503D21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,10 +156,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니 담기 - 옵션의 재고가 부족한 경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장바구니 담기 - 옵션가격이 판매자에 의해 변경된 경우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,6 +189,10 @@
   </si>
   <si>
     <t>상품수정 - 상품등록 조건을 만족해야 함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니 담기 - 옵션의 재고를 초과하는 경우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF758019-3106-4C82-A659-4C7DE0788447}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -743,7 +743,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -775,7 +775,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -783,7 +783,7 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -791,7 +791,7 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +807,7 @@
         <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -823,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>